<commit_message>
make behavioral analysis sensitive to number of trials
</commit_message>
<xml_diff>
--- a/code/istart_covariates_1aug22_modelready.xlsx
+++ b/code/istart_covariates_1aug22_modelready.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/Documents_Air/GitHub/istart-socdoors/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2732C1A-0F15-D145-B3EE-64243F285CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7528D2-7C9C-B64C-9079-EC274D03717D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="680" windowWidth="21400" windowHeight="15560" xr2:uid="{487F9E33-39B8-B043-9A6F-9C42D7109D31}"/>
+    <workbookView xWindow="5620" yWindow="540" windowWidth="21400" windowHeight="15560" xr2:uid="{487F9E33-39B8-B043-9A6F-9C42D7109D31}"/>
   </bookViews>
   <sheets>
     <sheet name="model-2_doors" sheetId="2" r:id="rId1"/>
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A475D1-7955-4D4C-B059-3A9B6F1866A0}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1256,32 +1256,32 @@
         <v>-7.1896298776812273</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
         <v>1255</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
         <v>0.93878051856977496</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>-0.12840687021826899</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>-0.5777777777777775</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>-8.0879012345678998</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>0.30544214264179498</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="2">
         <v>-0.59321351452381177</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="2">
         <v>0.87855582996227577</v>
       </c>
     </row>
@@ -1836,32 +1836,32 @@
         <v>-2.0734112184381801</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42">
+    <row r="42" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
         <v>3199</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2">
         <v>-1.1953814910827301</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="2">
         <v>1.2822248033022601</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>1.4222222222222225</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="2">
         <v>-6.3990123456790098</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="2">
         <v>-0.55422238147074898</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="2">
         <v>-1.2049632190891735</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="2">
         <v>6.8954175738068582</v>
       </c>
     </row>

</xml_diff>